<commit_message>
Aggiornamento gestione errore casi 28, 36, 44
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/D4CLIS/1.3/report-checklist.xlsx
+++ b/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/D4CLIS/1.3/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FSE\Validazione\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FSE\it-fse-accreditamento\GATEWAY\S1#111DEDALUS0000\DEDALUS_SPA\D4CLIS\1.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8540859D-CA18-40BE-A42E-5E5ADE40141D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F811C856-EE45-44E6-9B49-CC9899A33F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15750" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,8 +23,19 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">TestCases!$A$9:$T$374</definedName>
     <definedName name="filtro" localSheetId="2">TestCases!$A$9:$S$203</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataSignature="AMtx7mhUlYP9yzNmk4f07XMJovPPUaqOhw=="/>
     </ext>
@@ -64,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2116" uniqueCount="862">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2116" uniqueCount="864">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4543,6 +4554,14 @@
   </si>
   <si>
     <t>2023-05-08T10:43:14Z</t>
+  </si>
+  <si>
+    <t>In questa occorrenza viene memorizzato il messaggio di errore che proviene dal sevizio di validazione per analisi successiva in backoffice.
+L'errore ricevuto non preclude la produzione (e se presente firma) del referto in laboratorio e la notifica al repository aziendale (se presente)</t>
+  </si>
+  <si>
+    <t>In caso di timeout viene effettuata una retry per un numero di volte configurabile e ad intervalli di tempo configurabili.
+Superato il numero massimo di retry viene memorizzato il messaggio di errore, l'errore ricevuto non preclude la produzione (e se presente firma) del referto in laboratorio e la notifica al repository aziendale (se presente)</t>
   </si>
 </sst>
 </file>
@@ -6481,10 +6500,10 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="E186" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B190" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="J189" sqref="J189"/>
+      <selection pane="bottomRight" activeCell="P227" sqref="P227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -13614,7 +13633,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="211" spans="1:20" ht="150.75" thickBot="1">
+    <row r="211" spans="1:20" ht="180.75" thickBot="1">
       <c r="A211" s="20">
         <v>28</v>
       </c>
@@ -13659,7 +13678,7 @@
         <v>489</v>
       </c>
       <c r="P211" s="25" t="s">
-        <v>838</v>
+        <v>862</v>
       </c>
       <c r="Q211" s="25"/>
       <c r="R211" s="26"/>
@@ -13906,7 +13925,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="219" spans="1:20" ht="165.75" thickBot="1">
+    <row r="219" spans="1:20" ht="180.75" thickBot="1">
       <c r="A219" s="20">
         <v>36</v>
       </c>
@@ -13951,7 +13970,7 @@
         <v>489</v>
       </c>
       <c r="P219" s="25" t="s">
-        <v>838</v>
+        <v>862</v>
       </c>
       <c r="Q219" s="25"/>
       <c r="R219" s="26"/>
@@ -14198,7 +14217,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="227" spans="1:20" ht="90.75" thickBot="1">
+    <row r="227" spans="1:20" ht="210.75" thickBot="1">
       <c r="A227" s="20">
         <v>44</v>
       </c>
@@ -14237,7 +14256,7 @@
         <v>489</v>
       </c>
       <c r="P227" s="25" t="s">
-        <v>838</v>
+        <v>863</v>
       </c>
       <c r="Q227" s="25"/>
       <c r="R227" s="26"/>

</xml_diff>